<commit_message>
explore data page update to year selector
</commit_message>
<xml_diff>
--- a/gatsby-site/src/data/federal_disbursements.xlsx
+++ b/gatsby-site/src/data/federal_disbursements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="15">
   <si>
     <t>Offshore</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>American Indian Tribes</t>
-  </si>
-  <si>
-    <t>onshore</t>
   </si>
   <si>
     <t>Reclamation</t>
@@ -424,7 +421,7 @@
   <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,16 +434,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -454,7 +451,7 @@
         <v>2014</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
@@ -468,7 +465,7 @@
         <v>2014</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>0</v>
@@ -513,7 +510,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3">
         <v>1146119618.6800001</v>
@@ -527,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" s="3">
         <v>194422815.68000001</v>
@@ -538,10 +535,10 @@
         <v>2014</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D8" s="3">
         <v>1766192706.99</v>
@@ -552,10 +549,10 @@
         <v>2014</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3">
         <v>2187978477.289999</v>
@@ -569,7 +566,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10" s="3">
         <v>551361445.35000098</v>
@@ -580,10 +577,10 @@
         <v>2014</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="5">
         <v>34101233.449999996</v>
@@ -594,10 +591,10 @@
         <v>2014</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3">
         <v>877818.12</v>
@@ -611,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="3">
         <v>3362351.09</v>
@@ -622,10 +619,10 @@
         <v>2014</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1">
         <v>4297873.41</v>
@@ -639,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="3">
         <v>625237.05000000005</v>
@@ -650,7 +647,7 @@
         <v>2015</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
@@ -664,7 +661,7 @@
         <v>2015</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
@@ -709,7 +706,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20" s="3">
         <v>852729350.94000006</v>
@@ -723,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21" s="3">
         <v>153527706.74000001</v>
@@ -734,10 +731,10 @@
         <v>2015</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22" s="3">
         <v>1398152074.75</v>
@@ -748,10 +745,10 @@
         <v>2015</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" s="3">
         <v>1814559610.5500016</v>
@@ -765,7 +762,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24" s="3">
         <v>430430343.81</v>
@@ -776,10 +773,10 @@
         <v>2015</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" s="5">
         <v>22146231.09</v>
@@ -790,10 +787,10 @@
         <v>2015</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" s="3">
         <v>95097.14</v>
@@ -807,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" s="3">
         <v>1399279.23</v>
@@ -818,10 +815,10 @@
         <v>2015</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" s="4">
         <v>2441209.0299999998</v>
@@ -835,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29" s="3">
         <v>1232665.94</v>
@@ -846,7 +843,7 @@
         <v>2016</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>0</v>
@@ -891,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D33" s="3">
         <v>560416155.14999998</v>
@@ -905,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34" s="3">
         <v>91256204.899999902</v>
@@ -916,10 +913,10 @@
         <v>2016</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D35" s="3">
         <v>1009078894.55999</v>
@@ -930,10 +927,10 @@
         <v>2016</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D36" s="3">
         <v>1316110457.9400005</v>
@@ -947,7 +944,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D37" s="3">
         <v>336570856.33999997</v>
@@ -958,10 +955,10 @@
         <v>2016</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38" s="5">
         <v>10774005.139999999</v>
@@ -972,10 +969,10 @@
         <v>2016</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D39" s="3">
         <v>342654.53</v>
@@ -989,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40" s="3">
         <v>2352673.85</v>
@@ -1000,10 +997,10 @@
         <v>2016</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41" s="4">
         <v>314205.13</v>
@@ -1017,7 +1014,7 @@
         <v>2</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D42" s="3">
         <v>1370611.67</v>
@@ -1028,7 +1025,7 @@
         <v>2017</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>0</v>
@@ -1042,7 +1039,7 @@
         <v>2017</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>0</v>
@@ -1087,7 +1084,7 @@
         <v>3</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D47" s="3">
         <v>675788643.34000051</v>
@@ -1101,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D48" s="3">
         <v>111303696.5900002</v>
@@ -1112,10 +1109,10 @@
         <v>2017</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D49" s="3">
         <v>1142376548.9999981</v>
@@ -1126,10 +1123,10 @@
         <v>2017</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D50" s="3">
         <v>1427205063.6700013</v>
@@ -1143,7 +1140,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D51" s="3">
         <v>496239191.86999989</v>
@@ -1154,10 +1151,10 @@
         <v>2017</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D52" s="5">
         <v>10320922.99</v>
@@ -1168,10 +1165,10 @@
         <v>2017</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D53" s="3">
         <v>66982984.719999731</v>
@@ -1185,7 +1182,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D54" s="3">
         <v>77617720.029998511</v>
@@ -1196,10 +1193,10 @@
         <v>2017</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D55" s="4">
         <v>957032.2899999998</v>
@@ -1213,7 +1210,7 @@
         <v>2</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D56" s="3">
         <v>267931822.86000061</v>

</xml_diff>